<commit_message>
renamed and consolidated some parts names
</commit_message>
<xml_diff>
--- a/Nestbox_v3/BOM_Nestbox_v2.xlsx
+++ b/Nestbox_v3/BOM_Nestbox_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="16720" yWindow="-20" windowWidth="16800" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_Nestbox_v2.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="228">
   <si>
     <t>Source:</t>
   </si>
@@ -661,9 +661,6 @@
   </si>
   <si>
     <t>silkscreen illegible</t>
-  </si>
-  <si>
-    <t>consolidate with other inductor possible?</t>
   </si>
   <si>
     <t>??? Are the component names inverted???</t>
@@ -712,7 +709,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -755,6 +752,18 @@
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="6"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -832,7 +841,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -869,8 +878,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -885,8 +916,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="36">
+  <cellStyles count="58">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -906,6 +939,17 @@
     <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -922,6 +966,17 @@
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1256,16 +1311,17 @@
   </sheetPr>
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="B36" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="44" customWidth="1"/>
     <col min="4" max="4" width="23.6640625" customWidth="1"/>
-    <col min="7" max="9" width="0" hidden="1" customWidth="1"/>
-    <col min="10" max="11" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="26.33203125" customWidth="1"/>
+    <col min="8" max="8" width="7.83203125" customWidth="1"/>
+    <col min="9" max="12" width="8.6640625" customWidth="1"/>
     <col min="13" max="13" width="43.1640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1375,7 +1431,7 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="12" t="s">
         <v>210</v>
       </c>
     </row>
@@ -1543,7 +1599,7 @@
       <c r="L14" s="3">
         <v>302010067</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="M14" s="12" t="s">
         <v>211</v>
       </c>
     </row>
@@ -1601,8 +1657,8 @@
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
-      <c r="M16" s="4" t="s">
-        <v>228</v>
+      <c r="M16" s="12" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -1630,8 +1686,8 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
-      <c r="M17" s="4" t="s">
-        <v>225</v>
+      <c r="M17" s="13" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -1688,7 +1744,7 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
-      <c r="M19" s="4" t="s">
+      <c r="M19" s="12" t="s">
         <v>213</v>
       </c>
     </row>
@@ -2105,9 +2161,7 @@
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
-      <c r="M34" s="4" t="s">
-        <v>214</v>
-      </c>
+      <c r="M34" s="4"/>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="8">
@@ -2136,8 +2190,8 @@
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
-      <c r="M35" s="4" t="s">
-        <v>215</v>
+      <c r="M35" s="12" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -2396,7 +2450,7 @@
         <v>127</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>128</v>
@@ -2410,8 +2464,8 @@
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
-      <c r="M45" s="4" t="s">
-        <v>217</v>
+      <c r="M45" s="12" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="46" spans="1:13">
@@ -2425,7 +2479,7 @@
         <v>192</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>128</v>
@@ -2439,8 +2493,8 @@
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
-      <c r="M46" s="4" t="s">
-        <v>220</v>
+      <c r="M46" s="12" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="47" spans="1:13">
@@ -2481,7 +2535,7 @@
         <v>132</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>128</v>
@@ -2508,7 +2562,7 @@
         <v>133</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>128</v>
@@ -2580,8 +2634,8 @@
       <c r="L51" s="3">
         <v>301020022</v>
       </c>
-      <c r="M51" s="4" t="s">
-        <v>216</v>
+      <c r="M51" s="12" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="52" spans="1:13">
@@ -2663,8 +2717,8 @@
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
-      <c r="M54" s="4" t="s">
-        <v>221</v>
+      <c r="M54" s="12" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="55" spans="1:13">
@@ -2705,7 +2759,7 @@
         <v>197</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>128</v>
@@ -2804,8 +2858,8 @@
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
-      <c r="M59" s="4" t="s">
-        <v>226</v>
+      <c r="M59" s="12" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="60" spans="1:13">
@@ -2819,7 +2873,7 @@
         <v>200</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>128</v>
@@ -2846,7 +2900,7 @@
         <v>201</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>128</v>
@@ -2918,8 +2972,8 @@
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
-      <c r="M63" s="4" t="s">
-        <v>227</v>
+      <c r="M63" s="12" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="64" spans="1:13">

</xml_diff>